<commit_message>
Changed some input images to have more favourable dimensions
</commit_message>
<xml_diff>
--- a/Data/CPU/CPU data collection.xlsx
+++ b/Data/CPU/CPU data collection.xlsx
@@ -32,16 +32,7 @@
     <t>256x256</t>
   </si>
   <si>
-    <t>512x640</t>
-  </si>
-  <si>
     <t>1024x1024</t>
-  </si>
-  <si>
-    <t>1536x1920</t>
-  </si>
-  <si>
-    <t>5014x3342</t>
   </si>
   <si>
     <t>Image dimensions</t>
@@ -66,6 +57,15 @@
   </si>
   <si>
     <t>Openmp simd (todo)</t>
+  </si>
+  <si>
+    <t>512x512</t>
+  </si>
+  <si>
+    <t>2048x2048</t>
+  </si>
+  <si>
+    <t>4096x4096</t>
   </si>
 </sst>
 </file>
@@ -227,16 +227,16 @@
                   <c:v>256x256</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>512x640</c:v>
+                  <c:v>512x512</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1024x1024</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1536x1920</c:v>
+                  <c:v>2048x2048</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5014x3342</c:v>
+                  <c:v>4096x4096</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -279,11 +279,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2108480608"/>
-        <c:axId val="-2108478976"/>
+        <c:axId val="-1334943488"/>
+        <c:axId val="-1334940768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2108480608"/>
+        <c:axId val="-1334943488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -326,7 +326,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2108478976"/>
+        <c:crossAx val="-1334940768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -334,7 +334,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108478976"/>
+        <c:axId val="-1334940768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -385,7 +385,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2108480608"/>
+        <c:crossAx val="-1334943488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -548,16 +548,16 @@
                   <c:v>256x256</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>512x640</c:v>
+                  <c:v>512x512</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1024x1024</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1536x1920</c:v>
+                  <c:v>2048x2048</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5014x3342</c:v>
+                  <c:v>4096x4096</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -600,11 +600,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2047233024"/>
-        <c:axId val="-2047239008"/>
+        <c:axId val="-1073649248"/>
+        <c:axId val="-1073645984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2047233024"/>
+        <c:axId val="-1073649248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -647,7 +647,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2047239008"/>
+        <c:crossAx val="-1073645984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -655,7 +655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2047239008"/>
+        <c:axId val="-1073645984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -706,7 +706,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2047233024"/>
+        <c:crossAx val="-1073649248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -857,16 +857,16 @@
                   <c:v>256x256</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>512x640</c:v>
+                  <c:v>512x512</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1024x1024</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1536x1920</c:v>
+                  <c:v>2048x2048</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5014x3342</c:v>
+                  <c:v>4096x4096</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -909,11 +909,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2108477344"/>
-        <c:axId val="-2108476800"/>
+        <c:axId val="-1073654688"/>
+        <c:axId val="-1073657952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2108477344"/>
+        <c:axId val="-1073654688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,7 +956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2108476800"/>
+        <c:crossAx val="-1073657952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -964,7 +964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108476800"/>
+        <c:axId val="-1073657952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1015,7 +1015,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2108477344"/>
+        <c:crossAx val="-1073654688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3054,7 +3054,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3068,28 +3068,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3140,7 +3140,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>6.0193299999999998E-3</v>
@@ -3160,7 +3160,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>6.2482800000000002E-3</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>6.12665E-3</v>
@@ -3203,7 +3203,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>6.1549400000000002E-3</v>

</xml_diff>

<commit_message>
GPU routine completed with timers.
</commit_message>
<xml_diff>
--- a/Data/CPU/CPU data collection.xlsx
+++ b/Data/CPU/CPU data collection.xlsx
@@ -287,11 +287,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-706283040"/>
-        <c:axId val="-706279776"/>
+        <c:axId val="-1557955568"/>
+        <c:axId val="-1557967536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-706283040"/>
+        <c:axId val="-1557955568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,7 +398,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-706279776"/>
+        <c:crossAx val="-1557967536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -406,7 +406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-706279776"/>
+        <c:axId val="-1557967536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,7 +499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-706283040"/>
+        <c:crossAx val="-1557955568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -583,11 +583,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Tiling</a:t>
+              <a:t>Tiling of the outmost</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> </a:t>
+              <a:t> two loops </a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -597,8 +597,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.4011596675415573"/>
-          <c:y val="2.7777777777777776E-2"/>
+          <c:x val="0.28244817969191544"/>
+          <c:y val="3.2289776621283676E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -714,11 +714,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-706278688"/>
-        <c:axId val="-706291200"/>
+        <c:axId val="-1556140304"/>
+        <c:axId val="-1556135408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-706278688"/>
+        <c:axId val="-1556140304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,7 +822,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-706291200"/>
+        <c:crossAx val="-1556135408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -830,7 +830,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-706291200"/>
+        <c:axId val="-1556135408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +937,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-706278688"/>
+        <c:crossAx val="-1556140304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1140,11 +1140,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-706284672"/>
-        <c:axId val="-706277600"/>
+        <c:axId val="-1556136496"/>
+        <c:axId val="-1556139760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-706284672"/>
+        <c:axId val="-1556136496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1243,7 +1243,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-706277600"/>
+        <c:crossAx val="-1556139760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1251,7 +1251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-706277600"/>
+        <c:axId val="-1556139760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1358,7 +1358,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-706284672"/>
+        <c:crossAx val="-1556136496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1561,11 +1561,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-712879520"/>
-        <c:axId val="-712878976"/>
+        <c:axId val="-1556138672"/>
+        <c:axId val="-1556137040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-712879520"/>
+        <c:axId val="-1556138672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1669,7 +1669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-712878976"/>
+        <c:crossAx val="-1556137040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1677,7 +1677,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-712878976"/>
+        <c:axId val="-1556137040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1784,7 +1784,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-712879520"/>
+        <c:crossAx val="-1556138672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1987,11 +1987,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-292645680"/>
-        <c:axId val="-292648400"/>
+        <c:axId val="-1556132688"/>
+        <c:axId val="-1556131600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-292645680"/>
+        <c:axId val="-1556132688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2090,7 +2090,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-292648400"/>
+        <c:crossAx val="-1556131600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2098,7 +2098,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-292648400"/>
+        <c:axId val="-1556131600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2205,7 +2205,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-292645680"/>
+        <c:crossAx val="-1556132688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2408,11 +2408,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-773448752"/>
-        <c:axId val="-773447120"/>
+        <c:axId val="-1556131056"/>
+        <c:axId val="-1556130512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-773448752"/>
+        <c:axId val="-1556131056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2511,7 +2511,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773447120"/>
+        <c:crossAx val="-1556130512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2519,7 +2519,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-773447120"/>
+        <c:axId val="-1556130512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2626,7 +2626,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-773448752"/>
+        <c:crossAx val="-1556131056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2829,11 +2829,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-288391888"/>
-        <c:axId val="-288407120"/>
+        <c:axId val="-1556129968"/>
+        <c:axId val="-1282984048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-288391888"/>
+        <c:axId val="-1556129968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2932,7 +2932,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-288407120"/>
+        <c:crossAx val="-1282984048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2940,7 +2940,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-288407120"/>
+        <c:axId val="-1282984048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3047,7 +3047,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-288391888"/>
+        <c:crossAx val="-1556129968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3135,7 +3135,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> + AVX + regblock</a:t>
+              <a:t> + AVX + Register blocking factor 2</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -3255,11 +3255,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-288404400"/>
-        <c:axId val="-288406576"/>
+        <c:axId val="-1282985680"/>
+        <c:axId val="-1282990032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-288404400"/>
+        <c:axId val="-1282985680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3358,7 +3358,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-288406576"/>
+        <c:crossAx val="-1282990032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3366,7 +3366,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-288406576"/>
+        <c:axId val="-1282990032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3473,7 +3473,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-288404400"/>
+        <c:crossAx val="-1282985680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8376,8 +8376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added final routines for testing for CPU
</commit_message>
<xml_diff>
--- a/Data/CPU/CPU data collection.xlsx
+++ b/Data/CPU/CPU data collection.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="30">
   <si>
     <t>100x100</t>
   </si>
@@ -78,6 +79,42 @@
   </si>
   <si>
     <t>Tiling(32)</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Regblock factors</t>
+  </si>
+  <si>
+    <t>result 1</t>
+  </si>
+  <si>
+    <t>result 2</t>
+  </si>
+  <si>
+    <t>result 3</t>
+  </si>
+  <si>
+    <t>Tiling factors</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>Parallel threads</t>
+  </si>
+  <si>
+    <t>Unroll inner loop</t>
+  </si>
+  <si>
+    <t>highest</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>Parallel-8AvxRegblock-2tiled-64</t>
   </si>
 </sst>
 </file>
@@ -287,11 +324,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1557955568"/>
-        <c:axId val="-1557967536"/>
+        <c:axId val="1098448704"/>
+        <c:axId val="1098450336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1557955568"/>
+        <c:axId val="1098448704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,7 +435,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1557967536"/>
+        <c:crossAx val="1098450336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -406,7 +443,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1557967536"/>
+        <c:axId val="1098450336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,7 +536,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1557955568"/>
+        <c:crossAx val="1098448704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -714,11 +751,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1556140304"/>
-        <c:axId val="-1556135408"/>
+        <c:axId val="1098450880"/>
+        <c:axId val="1098445440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1556140304"/>
+        <c:axId val="1098450880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,7 +859,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1556135408"/>
+        <c:crossAx val="1098445440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -830,7 +867,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1556135408"/>
+        <c:axId val="1098445440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +974,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1556140304"/>
+        <c:crossAx val="1098450880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1140,11 +1177,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1556136496"/>
-        <c:axId val="-1556139760"/>
+        <c:axId val="1098454144"/>
+        <c:axId val="1098451968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1556136496"/>
+        <c:axId val="1098454144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1243,7 +1280,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1556139760"/>
+        <c:crossAx val="1098451968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1251,7 +1288,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1556139760"/>
+        <c:axId val="1098451968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1358,7 +1395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1556136496"/>
+        <c:crossAx val="1098454144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1561,11 +1598,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1556138672"/>
-        <c:axId val="-1556137040"/>
+        <c:axId val="1098454688"/>
+        <c:axId val="1098452512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1556138672"/>
+        <c:axId val="1098454688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1669,7 +1706,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1556137040"/>
+        <c:crossAx val="1098452512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1677,7 +1714,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1556137040"/>
+        <c:axId val="1098452512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1784,7 +1821,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1556138672"/>
+        <c:crossAx val="1098454688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1987,11 +2024,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1556132688"/>
-        <c:axId val="-1556131600"/>
+        <c:axId val="1098455232"/>
+        <c:axId val="1098459584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1556132688"/>
+        <c:axId val="1098455232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2090,7 +2127,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1556131600"/>
+        <c:crossAx val="1098459584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2098,7 +2135,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1556131600"/>
+        <c:axId val="1098459584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2205,7 +2242,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1556132688"/>
+        <c:crossAx val="1098455232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2408,11 +2445,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1556131056"/>
-        <c:axId val="-1556130512"/>
+        <c:axId val="1098444352"/>
+        <c:axId val="1098455776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1556131056"/>
+        <c:axId val="1098444352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2511,7 +2548,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1556130512"/>
+        <c:crossAx val="1098455776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2519,7 +2556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1556130512"/>
+        <c:axId val="1098455776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2626,7 +2663,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1556131056"/>
+        <c:crossAx val="1098444352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2829,11 +2866,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1556129968"/>
-        <c:axId val="-1282984048"/>
+        <c:axId val="1098456864"/>
+        <c:axId val="1098457408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1556129968"/>
+        <c:axId val="1098456864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2932,7 +2969,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1282984048"/>
+        <c:crossAx val="1098457408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2940,7 +2977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1282984048"/>
+        <c:axId val="1098457408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3047,7 +3084,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1556129968"/>
+        <c:crossAx val="1098456864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3255,11 +3292,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1282985680"/>
-        <c:axId val="-1282990032"/>
+        <c:axId val="1098457952"/>
+        <c:axId val="1098446528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1282985680"/>
+        <c:axId val="1098457952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3358,7 +3395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1282990032"/>
+        <c:crossAx val="1098446528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3366,7 +3403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1282990032"/>
+        <c:axId val="1098446528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3473,7 +3510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1282985680"/>
+        <c:crossAx val="1098457952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8376,8 +8413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="Q43" sqref="Q43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8609,4 +8646,2000 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H110"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J110" sqref="J110"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>9126700</v>
+      </c>
+      <c r="E3" s="1">
+        <v>9134930</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9126930</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="0">AVERAGE(D3:F3)</f>
+        <v>9129520</v>
+      </c>
+      <c r="H3">
+        <f>MAX(D3:F3)</f>
+        <v>9134930</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8843160</v>
+      </c>
+      <c r="E4" s="1">
+        <v>9075980</v>
+      </c>
+      <c r="F4" s="1">
+        <v>9121520</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>9013553.333333334</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H67" si="1">MAX(D4:F4)</f>
+        <v>9121520</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>9096280</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9085920</v>
+      </c>
+      <c r="F5" s="1">
+        <v>9083690</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>9088630</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>9096280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>9144200</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9039660</v>
+      </c>
+      <c r="F6" s="1">
+        <v>9140260</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>9108040</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>9144200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>9108090</v>
+      </c>
+      <c r="E7" s="1">
+        <v>9085520</v>
+      </c>
+      <c r="F7" s="1">
+        <v>9107740</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>9100450</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>9108090</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>9157500</v>
+      </c>
+      <c r="E8" s="1">
+        <v>9037490</v>
+      </c>
+      <c r="F8" s="1">
+        <v>9142190</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>9112393.333333334</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>9157500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>9657140</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9707320</v>
+      </c>
+      <c r="F11" s="1">
+        <v>9713760</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>9692740</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>9713760</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>9721690</v>
+      </c>
+      <c r="E12" s="1">
+        <v>9720940</v>
+      </c>
+      <c r="F12" s="1">
+        <v>9700380</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>9714336.666666666</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>9721690</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1">
+        <v>9710910</v>
+      </c>
+      <c r="E13" s="1">
+        <v>9696770</v>
+      </c>
+      <c r="F13" s="1">
+        <v>9663610</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>9690430</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>9710910</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>9672560</v>
+      </c>
+      <c r="E14" s="1">
+        <v>9675200</v>
+      </c>
+      <c r="F14" s="1">
+        <v>9662620</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>9670126.666666666</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>9675200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1">
+        <v>9734340</v>
+      </c>
+      <c r="E15" s="1">
+        <v>9752890</v>
+      </c>
+      <c r="F15" s="1">
+        <v>9669120</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>9718783.333333334</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>9752890</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1">
+        <v>9726180</v>
+      </c>
+      <c r="E16" s="1">
+        <v>9699860</v>
+      </c>
+      <c r="F16" s="1">
+        <v>9782160</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>9736066.666666666</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>9782160</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>16442400</v>
+      </c>
+      <c r="E20" s="1">
+        <v>16093200</v>
+      </c>
+      <c r="F20" s="1">
+        <v>16093200</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>16209600</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>16442400</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>16244500</v>
+      </c>
+      <c r="E21" s="1">
+        <v>16512000</v>
+      </c>
+      <c r="F21" s="1">
+        <v>16512000</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>16422833.333333334</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>16512000</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1">
+        <v>16554100</v>
+      </c>
+      <c r="E22" s="1">
+        <v>16271900</v>
+      </c>
+      <c r="F22" s="1">
+        <v>16271900</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>16365966.666666666</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>16554100</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>16323600</v>
+      </c>
+      <c r="E23" s="1">
+        <v>16560000</v>
+      </c>
+      <c r="F23" s="1">
+        <v>16560000</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>16481200</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>16560000</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1">
+        <v>16502300</v>
+      </c>
+      <c r="E24" s="1">
+        <v>16353500</v>
+      </c>
+      <c r="F24" s="1">
+        <v>16353500</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>16403100</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>16502300</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1">
+        <v>16328100</v>
+      </c>
+      <c r="E25" s="1">
+        <v>16289000</v>
+      </c>
+      <c r="F25" s="1">
+        <v>16289000</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>16302033.333333334</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>16328100</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>16257000</v>
+      </c>
+      <c r="E27" s="1">
+        <v>16470000</v>
+      </c>
+      <c r="F27" s="1">
+        <v>16345300</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>16357433.333333334</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>16470000</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>16690000</v>
+      </c>
+      <c r="E28" s="1">
+        <v>16731600</v>
+      </c>
+      <c r="F28" s="1">
+        <v>16759800</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>16727133.333333334</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>16759800</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1">
+        <v>16836200</v>
+      </c>
+      <c r="E29" s="1">
+        <v>16883200</v>
+      </c>
+      <c r="F29" s="1">
+        <v>16869300</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>16862900</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>16883200</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>16920200</v>
+      </c>
+      <c r="E30" s="1">
+        <v>16937900</v>
+      </c>
+      <c r="F30" s="1">
+        <v>16763300</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>16873800</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>16937900</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1">
+        <v>16796300</v>
+      </c>
+      <c r="E31" s="1">
+        <v>17094800</v>
+      </c>
+      <c r="F31" s="1">
+        <v>16800900</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>16897333.333333332</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>17094800</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="1">
+        <v>17095200</v>
+      </c>
+      <c r="E32" s="1">
+        <v>16588200</v>
+      </c>
+      <c r="F32" s="1">
+        <v>17031800</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>16905066.666666668</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>17095200</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>7750480</v>
+      </c>
+      <c r="E34" s="1">
+        <v>7737330</v>
+      </c>
+      <c r="F34" s="1">
+        <v>7759670</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>7749160</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>7759670</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>7810020</v>
+      </c>
+      <c r="E35" s="1">
+        <v>7794300</v>
+      </c>
+      <c r="F35" s="1">
+        <v>7838790</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>7814370</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>7838790</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1">
+        <v>7826040</v>
+      </c>
+      <c r="E36" s="1">
+        <v>7818210</v>
+      </c>
+      <c r="F36" s="1">
+        <v>7851910</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>7832053.333333333</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>7851910</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>7831990</v>
+      </c>
+      <c r="E37" s="1">
+        <v>7849070</v>
+      </c>
+      <c r="F37" s="1">
+        <v>7814630</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>7831896.666666667</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>7849070</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="1">
+        <v>7835520</v>
+      </c>
+      <c r="E38" s="1">
+        <v>7859290</v>
+      </c>
+      <c r="F38" s="1">
+        <v>7854140</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>7849650</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="1"/>
+        <v>7859290</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="1">
+        <v>7889090</v>
+      </c>
+      <c r="E39" s="1">
+        <v>7813450</v>
+      </c>
+      <c r="F39" s="1">
+        <v>7914210</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>7872250</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>7914210</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1">
+        <v>9143810</v>
+      </c>
+      <c r="E43" s="1">
+        <v>9191380</v>
+      </c>
+      <c r="F43" s="1">
+        <v>9200160</v>
+      </c>
+      <c r="G43">
+        <f>AVERAGE(D43:F43)</f>
+        <v>9178450</v>
+      </c>
+      <c r="H43">
+        <f>MAX(D43:F43)</f>
+        <v>9200160</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <v>9095010</v>
+      </c>
+      <c r="E44" s="1">
+        <v>9216850</v>
+      </c>
+      <c r="F44" s="1">
+        <v>9208030</v>
+      </c>
+      <c r="G44">
+        <f>AVERAGE(D44:F44)</f>
+        <v>9173296.666666666</v>
+      </c>
+      <c r="H44">
+        <f>MAX(D44:F44)</f>
+        <v>9216850</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="1">
+        <v>9162840</v>
+      </c>
+      <c r="E45" s="1">
+        <v>9226130</v>
+      </c>
+      <c r="F45" s="1">
+        <v>9198990</v>
+      </c>
+      <c r="G45">
+        <f>AVERAGE(D45:F45)</f>
+        <v>9195986.666666666</v>
+      </c>
+      <c r="H45">
+        <f>MAX(D45:F45)</f>
+        <v>9226130</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>9127900</v>
+      </c>
+      <c r="E46" s="1">
+        <v>9215970</v>
+      </c>
+      <c r="F46" s="1">
+        <v>9196720</v>
+      </c>
+      <c r="G46">
+        <f>AVERAGE(D46:F46)</f>
+        <v>9180196.666666666</v>
+      </c>
+      <c r="H46">
+        <f>MAX(D46:F46)</f>
+        <v>9215970</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="1">
+        <v>9099890</v>
+      </c>
+      <c r="E47" s="1">
+        <v>9189830</v>
+      </c>
+      <c r="F47" s="1">
+        <v>9165760</v>
+      </c>
+      <c r="G47">
+        <f>AVERAGE(D47:F47)</f>
+        <v>9151826.666666666</v>
+      </c>
+      <c r="H47">
+        <f>MAX(D47:F47)</f>
+        <v>9189830</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="1">
+        <v>9176020</v>
+      </c>
+      <c r="E48" s="1">
+        <v>9176990</v>
+      </c>
+      <c r="F48" s="1">
+        <v>9152280</v>
+      </c>
+      <c r="G48">
+        <f>AVERAGE(D48:F48)</f>
+        <v>9168430</v>
+      </c>
+      <c r="H48">
+        <f>MAX(D48:F48)</f>
+        <v>9176990</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>9001990</v>
+      </c>
+      <c r="E50" s="1">
+        <v>9129980</v>
+      </c>
+      <c r="F50" s="1">
+        <v>9163350</v>
+      </c>
+      <c r="G50">
+        <f>AVERAGE(D50:F50)</f>
+        <v>9098440</v>
+      </c>
+      <c r="H50">
+        <f>MAX(D50:F50)</f>
+        <v>9163350</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
+        <v>9079620</v>
+      </c>
+      <c r="E51" s="1">
+        <v>9187840</v>
+      </c>
+      <c r="F51" s="1">
+        <v>9245190</v>
+      </c>
+      <c r="G51">
+        <f>AVERAGE(D51:F51)</f>
+        <v>9170883.333333334</v>
+      </c>
+      <c r="H51">
+        <f>MAX(D51:F51)</f>
+        <v>9245190</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="1">
+        <v>9048400</v>
+      </c>
+      <c r="E52" s="1">
+        <v>9188950</v>
+      </c>
+      <c r="F52" s="1">
+        <v>9212740</v>
+      </c>
+      <c r="G52">
+        <f>AVERAGE(D52:F52)</f>
+        <v>9150030</v>
+      </c>
+      <c r="H52">
+        <f>MAX(D52:F52)</f>
+        <v>9212740</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1">
+        <v>9021040</v>
+      </c>
+      <c r="E53" s="1">
+        <v>9150160</v>
+      </c>
+      <c r="F53" s="1">
+        <v>9184420</v>
+      </c>
+      <c r="G53">
+        <f>AVERAGE(D53:F53)</f>
+        <v>9118540</v>
+      </c>
+      <c r="H53">
+        <f>MAX(D53:F53)</f>
+        <v>9184420</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="1">
+        <v>8934700</v>
+      </c>
+      <c r="E54" s="1">
+        <v>9112570</v>
+      </c>
+      <c r="F54" s="1">
+        <v>9148270</v>
+      </c>
+      <c r="G54">
+        <f>AVERAGE(D54:F54)</f>
+        <v>9065180</v>
+      </c>
+      <c r="H54">
+        <f>MAX(D54:F54)</f>
+        <v>9148270</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="1">
+        <v>8984720</v>
+      </c>
+      <c r="E55" s="1">
+        <v>9139960</v>
+      </c>
+      <c r="F55" s="1">
+        <v>9091590</v>
+      </c>
+      <c r="G55">
+        <f>AVERAGE(D55:F55)</f>
+        <v>9072090</v>
+      </c>
+      <c r="H55">
+        <f>MAX(D55:F55)</f>
+        <v>9139960</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1">
+        <v>9234750</v>
+      </c>
+      <c r="E57" s="1">
+        <v>9155480</v>
+      </c>
+      <c r="F57" s="1">
+        <v>9194210</v>
+      </c>
+      <c r="G57">
+        <f>AVERAGE(D57:F57)</f>
+        <v>9194813.333333334</v>
+      </c>
+      <c r="H57">
+        <f>MAX(D57:F57)</f>
+        <v>9234750</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1">
+        <v>9214400</v>
+      </c>
+      <c r="E58" s="1">
+        <v>9234680</v>
+      </c>
+      <c r="F58" s="1">
+        <v>9216300</v>
+      </c>
+      <c r="G58">
+        <f>AVERAGE(D58:F58)</f>
+        <v>9221793.333333334</v>
+      </c>
+      <c r="H58">
+        <f>MAX(D58:F58)</f>
+        <v>9234680</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="1">
+        <v>9222910</v>
+      </c>
+      <c r="E59" s="1">
+        <v>9211310</v>
+      </c>
+      <c r="F59" s="1">
+        <v>9218380</v>
+      </c>
+      <c r="G59">
+        <f>AVERAGE(D59:F59)</f>
+        <v>9217533.333333334</v>
+      </c>
+      <c r="H59">
+        <f>MAX(D59:F59)</f>
+        <v>9222910</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" s="1">
+        <v>9152170</v>
+      </c>
+      <c r="E60" s="1">
+        <v>9135550</v>
+      </c>
+      <c r="F60" s="1">
+        <v>9143960</v>
+      </c>
+      <c r="G60">
+        <f t="shared" ref="G60:G123" si="2">AVERAGE(D60:F60)</f>
+        <v>9143893.333333334</v>
+      </c>
+      <c r="H60">
+        <f>MAX(D60:F60)</f>
+        <v>9152170</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="1">
+        <v>9042880</v>
+      </c>
+      <c r="E61" s="1">
+        <v>9076210</v>
+      </c>
+      <c r="F61" s="1">
+        <v>9026380</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="2"/>
+        <v>9048490</v>
+      </c>
+      <c r="H61">
+        <f t="shared" ref="H61:H124" si="3">MAX(D61:F61)</f>
+        <v>9076210</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="1">
+        <v>9015130</v>
+      </c>
+      <c r="E62" s="1">
+        <v>9078130</v>
+      </c>
+      <c r="F62" s="1">
+        <v>9014470</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="2"/>
+        <v>9035910</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="3"/>
+        <v>9078130</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1">
+        <v>9195870</v>
+      </c>
+      <c r="E64" s="1">
+        <v>9191270</v>
+      </c>
+      <c r="F64" s="1">
+        <v>9175810</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="2"/>
+        <v>9187650</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="3"/>
+        <v>9195870</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1">
+        <v>9207980</v>
+      </c>
+      <c r="E65" s="1">
+        <v>9224240</v>
+      </c>
+      <c r="F65" s="1">
+        <v>9225570</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="2"/>
+        <v>9219263.333333334</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="3"/>
+        <v>9225570</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="1">
+        <v>9217690</v>
+      </c>
+      <c r="E66" s="1">
+        <v>9209880</v>
+      </c>
+      <c r="F66" s="1">
+        <v>9215960</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="2"/>
+        <v>9214510</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="3"/>
+        <v>9217690</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="1">
+        <v>9194680</v>
+      </c>
+      <c r="E67" s="1">
+        <v>9202040</v>
+      </c>
+      <c r="F67" s="1">
+        <v>9209500</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="2"/>
+        <v>9202073.333333334</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="3"/>
+        <v>9209500</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="1">
+        <v>9182180</v>
+      </c>
+      <c r="E68" s="1">
+        <v>9199380</v>
+      </c>
+      <c r="F68" s="1">
+        <v>9236210</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="2"/>
+        <v>9205923.333333334</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="3"/>
+        <v>9236210</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="1">
+        <v>9259830</v>
+      </c>
+      <c r="E69" s="1">
+        <v>9141840</v>
+      </c>
+      <c r="F69" s="1">
+        <v>9255420</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="2"/>
+        <v>9219030</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="3"/>
+        <v>9259830</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1">
+        <v>41284900</v>
+      </c>
+      <c r="E73" s="1">
+        <v>42374700</v>
+      </c>
+      <c r="F73" s="1">
+        <v>42579800</v>
+      </c>
+      <c r="G73">
+        <f>AVERAGE(D73:F73)</f>
+        <v>42079800</v>
+      </c>
+      <c r="H73">
+        <f>MAX(D73:F73)</f>
+        <v>42579800</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>1</v>
+      </c>
+      <c r="D74" s="1">
+        <v>44537700</v>
+      </c>
+      <c r="E74" s="1">
+        <v>46597700</v>
+      </c>
+      <c r="F74" s="1">
+        <v>45419700</v>
+      </c>
+      <c r="G74">
+        <f>AVERAGE(D74:F74)</f>
+        <v>45518366.666666664</v>
+      </c>
+      <c r="H74">
+        <f>MAX(D74:F74)</f>
+        <v>46597700</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="1">
+        <v>45920200</v>
+      </c>
+      <c r="E75" s="1">
+        <v>47722200</v>
+      </c>
+      <c r="F75" s="1">
+        <v>46880400</v>
+      </c>
+      <c r="G75">
+        <f>AVERAGE(D75:F75)</f>
+        <v>46840933.333333336</v>
+      </c>
+      <c r="H75">
+        <f>MAX(D75:F75)</f>
+        <v>47722200</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="1">
+        <v>46523100</v>
+      </c>
+      <c r="E76" s="1">
+        <v>45636500</v>
+      </c>
+      <c r="F76" s="1">
+        <v>46810000</v>
+      </c>
+      <c r="G76">
+        <f>AVERAGE(D76:F76)</f>
+        <v>46323200</v>
+      </c>
+      <c r="H76">
+        <f>MAX(D76:F76)</f>
+        <v>46810000</v>
+      </c>
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="1">
+        <v>52016900</v>
+      </c>
+      <c r="E77" s="1">
+        <v>52939800</v>
+      </c>
+      <c r="F77" s="1">
+        <v>52096300</v>
+      </c>
+      <c r="G77">
+        <f>AVERAGE(D77:F77)</f>
+        <v>52351000</v>
+      </c>
+      <c r="H77">
+        <f>MAX(D77:F77)</f>
+        <v>52939800</v>
+      </c>
+    </row>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="1">
+        <v>57363800</v>
+      </c>
+      <c r="E78" s="1">
+        <v>57890200</v>
+      </c>
+      <c r="F78" s="1">
+        <v>57453100</v>
+      </c>
+      <c r="G78">
+        <f>AVERAGE(D78:F78)</f>
+        <v>57569033.333333336</v>
+      </c>
+      <c r="H78">
+        <f>MAX(D78:F78)</f>
+        <v>57890200</v>
+      </c>
+    </row>
+    <row r="80" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1">
+        <v>14246400</v>
+      </c>
+      <c r="E81" s="1">
+        <v>14309900</v>
+      </c>
+      <c r="F81" s="1">
+        <v>14333500</v>
+      </c>
+      <c r="G81">
+        <f>AVERAGE(D81:F81)</f>
+        <v>14296600</v>
+      </c>
+      <c r="H81">
+        <f>MAX(D81:F81)</f>
+        <v>14333500</v>
+      </c>
+    </row>
+    <row r="82" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D82" s="1">
+        <v>14532800</v>
+      </c>
+      <c r="E82" s="1">
+        <v>14489300</v>
+      </c>
+      <c r="F82" s="1">
+        <v>14502800</v>
+      </c>
+      <c r="G82">
+        <f>AVERAGE(D82:F82)</f>
+        <v>14508300</v>
+      </c>
+      <c r="H82">
+        <f>MAX(D82:F82)</f>
+        <v>14532800</v>
+      </c>
+    </row>
+    <row r="83" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="1">
+        <v>14537500</v>
+      </c>
+      <c r="E83" s="1">
+        <v>14525000</v>
+      </c>
+      <c r="F83" s="1">
+        <v>14552100</v>
+      </c>
+      <c r="G83">
+        <f>AVERAGE(D83:F83)</f>
+        <v>14538200</v>
+      </c>
+      <c r="H83">
+        <f>MAX(D83:F83)</f>
+        <v>14552100</v>
+      </c>
+    </row>
+    <row r="84" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" s="1">
+        <v>14573700</v>
+      </c>
+      <c r="E84" s="1">
+        <v>14540600</v>
+      </c>
+      <c r="F84" s="1">
+        <v>14551800</v>
+      </c>
+      <c r="G84">
+        <f>AVERAGE(D84:F84)</f>
+        <v>14555366.666666666</v>
+      </c>
+      <c r="H84">
+        <f>MAX(D84:F84)</f>
+        <v>14573700</v>
+      </c>
+    </row>
+    <row r="85" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" s="1">
+        <v>14522400</v>
+      </c>
+      <c r="E85" s="1">
+        <v>14592100</v>
+      </c>
+      <c r="F85" s="1">
+        <v>14438600</v>
+      </c>
+      <c r="G85">
+        <f>AVERAGE(D85:F85)</f>
+        <v>14517700</v>
+      </c>
+      <c r="H85">
+        <f>MAX(D85:F85)</f>
+        <v>14592100</v>
+      </c>
+    </row>
+    <row r="86" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="1">
+        <v>14444000</v>
+      </c>
+      <c r="E86" s="1">
+        <v>14691900</v>
+      </c>
+      <c r="F86" s="1">
+        <v>14418900</v>
+      </c>
+      <c r="G86">
+        <f>AVERAGE(D86:F86)</f>
+        <v>14518266.666666666</v>
+      </c>
+      <c r="H86">
+        <f>MAX(D86:F86)</f>
+        <v>14691900</v>
+      </c>
+    </row>
+    <row r="88" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="1">
+        <v>61752100</v>
+      </c>
+      <c r="E89" s="1">
+        <v>63054100</v>
+      </c>
+      <c r="F89" s="1">
+        <v>63283300</v>
+      </c>
+      <c r="G89">
+        <f>AVERAGE(D89:F89)</f>
+        <v>62696500</v>
+      </c>
+      <c r="H89">
+        <f>MAX(D89:F89)</f>
+        <v>63283300</v>
+      </c>
+    </row>
+    <row r="90" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" s="1">
+        <v>69888900</v>
+      </c>
+      <c r="E90" s="1">
+        <v>71418000</v>
+      </c>
+      <c r="F90" s="1">
+        <v>70734000</v>
+      </c>
+      <c r="G90">
+        <f>AVERAGE(D90:F90)</f>
+        <v>70680300</v>
+      </c>
+      <c r="H90">
+        <f>MAX(D90:F90)</f>
+        <v>71418000</v>
+      </c>
+    </row>
+    <row r="91" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="1">
+        <v>72543900</v>
+      </c>
+      <c r="E91" s="1">
+        <v>74284900</v>
+      </c>
+      <c r="F91" s="1">
+        <v>74278800</v>
+      </c>
+      <c r="G91">
+        <f>AVERAGE(D91:F91)</f>
+        <v>73702533.333333328</v>
+      </c>
+      <c r="H91">
+        <f>MAX(D91:F91)</f>
+        <v>74284900</v>
+      </c>
+    </row>
+    <row r="92" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" s="1">
+        <v>71835800</v>
+      </c>
+      <c r="E92" s="1">
+        <v>73906200</v>
+      </c>
+      <c r="F92" s="1">
+        <v>75274500</v>
+      </c>
+      <c r="G92">
+        <f>AVERAGE(D92:F92)</f>
+        <v>73672166.666666672</v>
+      </c>
+      <c r="H92">
+        <f>MAX(D92:F92)</f>
+        <v>75274500</v>
+      </c>
+    </row>
+    <row r="93" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" s="1">
+        <v>80027000</v>
+      </c>
+      <c r="E93" s="1">
+        <v>81565700</v>
+      </c>
+      <c r="F93" s="1">
+        <v>81021800</v>
+      </c>
+      <c r="G93">
+        <f>AVERAGE(D93:F93)</f>
+        <v>80871500</v>
+      </c>
+      <c r="H93">
+        <f>MAX(D93:F93)</f>
+        <v>81565700</v>
+      </c>
+    </row>
+    <row r="94" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" s="1">
+        <v>88334600</v>
+      </c>
+      <c r="E94" s="1">
+        <v>88739000</v>
+      </c>
+      <c r="F94" s="1">
+        <v>88306100</v>
+      </c>
+      <c r="G94">
+        <f>AVERAGE(D94:F94)</f>
+        <v>88459900</v>
+      </c>
+      <c r="H94">
+        <f>MAX(D94:F94)</f>
+        <v>88739000</v>
+      </c>
+    </row>
+    <row r="96" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="1">
+        <v>81127600</v>
+      </c>
+      <c r="E97" s="1">
+        <v>80729300</v>
+      </c>
+      <c r="F97" s="1">
+        <v>83752500</v>
+      </c>
+      <c r="G97">
+        <f>AVERAGE(D97:F97)</f>
+        <v>81869800</v>
+      </c>
+      <c r="H97">
+        <f>MAX(D97:F97)</f>
+        <v>83752500</v>
+      </c>
+    </row>
+    <row r="98" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" s="1">
+        <v>88974300</v>
+      </c>
+      <c r="E98" s="1">
+        <v>88674000</v>
+      </c>
+      <c r="F98" s="1">
+        <v>91529800</v>
+      </c>
+      <c r="G98">
+        <f>AVERAGE(D98:F98)</f>
+        <v>89726033.333333328</v>
+      </c>
+      <c r="H98">
+        <f>MAX(D98:F98)</f>
+        <v>91529800</v>
+      </c>
+    </row>
+    <row r="99" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="1">
+        <v>90067000</v>
+      </c>
+      <c r="E99" s="1">
+        <v>97747900</v>
+      </c>
+      <c r="F99" s="1">
+        <v>97655700</v>
+      </c>
+      <c r="G99">
+        <f>AVERAGE(D99:F99)</f>
+        <v>95156866.666666672</v>
+      </c>
+      <c r="H99">
+        <f>MAX(D99:F99)</f>
+        <v>97747900</v>
+      </c>
+    </row>
+    <row r="100" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" s="1">
+        <v>94745400</v>
+      </c>
+      <c r="E100" s="1">
+        <v>96545000</v>
+      </c>
+      <c r="F100" s="1">
+        <v>95837500</v>
+      </c>
+      <c r="G100">
+        <f>AVERAGE(D100:F100)</f>
+        <v>95709300</v>
+      </c>
+      <c r="H100">
+        <f>MAX(D100:F100)</f>
+        <v>96545000</v>
+      </c>
+    </row>
+    <row r="101" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" s="1">
+        <v>100417000</v>
+      </c>
+      <c r="E101" s="1">
+        <v>101128000</v>
+      </c>
+      <c r="F101" s="1">
+        <v>104031000</v>
+      </c>
+      <c r="G101">
+        <f>AVERAGE(D101:F101)</f>
+        <v>101858666.66666667</v>
+      </c>
+      <c r="H101">
+        <f>MAX(D101:F101)</f>
+        <v>104031000</v>
+      </c>
+    </row>
+    <row r="102" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102" s="1">
+        <v>112342000</v>
+      </c>
+      <c r="E102" s="1">
+        <v>113839000</v>
+      </c>
+      <c r="F102" s="1">
+        <v>113620000</v>
+      </c>
+      <c r="G102">
+        <f>AVERAGE(D102:F102)</f>
+        <v>113267000</v>
+      </c>
+      <c r="H102">
+        <f>MAX(D102:F102)</f>
+        <v>113839000</v>
+      </c>
+    </row>
+    <row r="104" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>0</v>
+      </c>
+      <c r="D105" s="1">
+        <v>24813000</v>
+      </c>
+      <c r="E105" s="1">
+        <v>24843000</v>
+      </c>
+      <c r="F105" s="1">
+        <v>24955400</v>
+      </c>
+      <c r="G105">
+        <f>AVERAGE(D105:F105)</f>
+        <v>24870466.666666668</v>
+      </c>
+      <c r="H105">
+        <f>MAX(D105:F105)</f>
+        <v>24955400</v>
+      </c>
+    </row>
+    <row r="106" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>1</v>
+      </c>
+      <c r="D106" s="1">
+        <v>50926500</v>
+      </c>
+      <c r="E106" s="1">
+        <v>50054100</v>
+      </c>
+      <c r="F106" s="1">
+        <v>51214500</v>
+      </c>
+      <c r="G106">
+        <f>AVERAGE(D106:F106)</f>
+        <v>50731700</v>
+      </c>
+      <c r="H106">
+        <f>MAX(D106:F106)</f>
+        <v>51214500</v>
+      </c>
+    </row>
+    <row r="107" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" s="1">
+        <v>95294900</v>
+      </c>
+      <c r="E107" s="1">
+        <v>94384600</v>
+      </c>
+      <c r="F107" s="1">
+        <v>92076600</v>
+      </c>
+      <c r="G107">
+        <f>AVERAGE(D107:F107)</f>
+        <v>93918700</v>
+      </c>
+      <c r="H107">
+        <f>MAX(D107:F107)</f>
+        <v>95294900</v>
+      </c>
+    </row>
+    <row r="108" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" s="1">
+        <v>95823500</v>
+      </c>
+      <c r="E108" s="1">
+        <v>97215700</v>
+      </c>
+      <c r="F108" s="1">
+        <v>92346000</v>
+      </c>
+      <c r="G108">
+        <f>AVERAGE(D108:F108)</f>
+        <v>95128400</v>
+      </c>
+      <c r="H108">
+        <f>MAX(D108:F108)</f>
+        <v>97215700</v>
+      </c>
+    </row>
+    <row r="109" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" s="1">
+        <v>101670000</v>
+      </c>
+      <c r="E109" s="1">
+        <v>101037000</v>
+      </c>
+      <c r="F109" s="1">
+        <v>100665000</v>
+      </c>
+      <c r="G109">
+        <f>AVERAGE(D109:F109)</f>
+        <v>101124000</v>
+      </c>
+      <c r="H109">
+        <f>MAX(D109:F109)</f>
+        <v>101670000</v>
+      </c>
+    </row>
+    <row r="110" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>8</v>
+      </c>
+      <c r="D110" s="1">
+        <v>112253000</v>
+      </c>
+      <c r="E110" s="1">
+        <v>112019000</v>
+      </c>
+      <c r="F110" s="1">
+        <v>113534000</v>
+      </c>
+      <c r="G110">
+        <f t="shared" ref="G110" si="4">AVERAGE(D110:F110)</f>
+        <v>112602000</v>
+      </c>
+      <c r="H110">
+        <f>MAX(D110:F110)</f>
+        <v>113534000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Upload of final data from tests.
</commit_message>
<xml_diff>
--- a/Data/CPU/CPU data collection.xlsx
+++ b/Data/CPU/CPU data collection.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="31">
   <si>
     <t>100x100</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Parallel-8AvxRegblock-2tiled-64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPU </t>
   </si>
 </sst>
 </file>
@@ -8650,10 +8653,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J110" sqref="J110"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K113" sqref="K113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10631,12 +10634,149 @@
         <v>113534000</v>
       </c>
       <c r="G110">
-        <f t="shared" ref="G110" si="4">AVERAGE(D110:F110)</f>
+        <f t="shared" ref="G110:G117" si="4">AVERAGE(D110:F110)</f>
         <v>112602000</v>
       </c>
       <c r="H110">
         <f>MAX(D110:F110)</f>
         <v>113534000</v>
+      </c>
+    </row>
+    <row r="111" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="112" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>0</v>
+      </c>
+      <c r="D112" s="1">
+        <v>179501000</v>
+      </c>
+      <c r="E112" s="1">
+        <v>323411000</v>
+      </c>
+      <c r="F112" s="1">
+        <v>64793800</v>
+      </c>
+      <c r="G112">
+        <f t="shared" si="4"/>
+        <v>189235266.66666666</v>
+      </c>
+      <c r="H112">
+        <f t="shared" ref="H111:H117" si="5">MAX(D112:F112)</f>
+        <v>323411000</v>
+      </c>
+    </row>
+    <row r="113" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>1</v>
+      </c>
+      <c r="D113" s="1">
+        <v>2278750000</v>
+      </c>
+      <c r="E113" s="1">
+        <v>2278110000</v>
+      </c>
+      <c r="F113" s="1">
+        <v>2193230000</v>
+      </c>
+      <c r="G113">
+        <f t="shared" si="4"/>
+        <v>2250030000</v>
+      </c>
+      <c r="H113">
+        <f t="shared" si="5"/>
+        <v>2278750000</v>
+      </c>
+    </row>
+    <row r="114" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" s="1">
+        <v>6085060000</v>
+      </c>
+      <c r="E114" s="1">
+        <v>5949220000</v>
+      </c>
+      <c r="F114" s="1">
+        <v>6130960000</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="4"/>
+        <v>6055080000</v>
+      </c>
+      <c r="H114">
+        <f t="shared" si="5"/>
+        <v>6130960000</v>
+      </c>
+    </row>
+    <row r="115" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>2</v>
+      </c>
+      <c r="D115" s="1">
+        <v>12674500000</v>
+      </c>
+      <c r="E115" s="1">
+        <v>12735100000</v>
+      </c>
+      <c r="F115" s="1">
+        <v>12643900000</v>
+      </c>
+      <c r="G115">
+        <f t="shared" si="4"/>
+        <v>12684500000</v>
+      </c>
+      <c r="H115">
+        <f t="shared" si="5"/>
+        <v>12735100000</v>
+      </c>
+    </row>
+    <row r="116" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>7</v>
+      </c>
+      <c r="D116" s="1">
+        <v>17063900000</v>
+      </c>
+      <c r="E116" s="1">
+        <v>17104600000</v>
+      </c>
+      <c r="F116" s="1">
+        <v>17112400000</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="4"/>
+        <v>17093633333.333334</v>
+      </c>
+      <c r="H116">
+        <f t="shared" si="5"/>
+        <v>17112400000</v>
+      </c>
+    </row>
+    <row r="117" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>8</v>
+      </c>
+      <c r="D117" s="1">
+        <v>1159260000</v>
+      </c>
+      <c r="E117" s="1">
+        <v>1163060000</v>
+      </c>
+      <c r="F117" s="1">
+        <v>1171950000</v>
+      </c>
+      <c r="G117">
+        <f t="shared" si="4"/>
+        <v>1164756666.6666667</v>
+      </c>
+      <c r="H117">
+        <f t="shared" si="5"/>
+        <v>1171950000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>